<commit_message>
Se suben los archivos de la practica 3, la clase Mezcla y sus mediciones de tiempo
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p3/Mediciones.xlsx
+++ b/src/main/java/algestudiante/p3/Mediciones.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\U N I\2º UNI\2do semestre\Algoritmia\Laboratorio\3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U N I\2º UNI\2do semestre\Algoritmia\Laboratorio\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{859EB3AC-DBF1-4778-A428-81F6B91B15D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>SUSTRACCION 2</t>
   </si>
@@ -109,12 +108,21 @@
   <si>
     <t>t(ms)</t>
   </si>
+  <si>
+    <t>MERGESORT ORDENADO</t>
+  </si>
+  <si>
+    <t>MERGESORT ORDENADO INVERSO</t>
+  </si>
+  <si>
+    <t>RAPIDO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +140,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -158,11 +174,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,6 +688,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -876,6 +894,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -993,6 +1012,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1589,6 +1609,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1770,6 +1791,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1892,6 +1914,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2047,6 +2070,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2222,6 +2246,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2344,6 +2369,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2499,6 +2525,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2686,6 +2713,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2803,6 +2831,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2870,6 +2899,1256 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1436206640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>MERGESORT ORDENADO</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$124:$A$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>31250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$124:$B$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7116</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33146</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F9E8-4AF2-BCA0-E16FDD36660A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2104560944"/>
+        <c:axId val="2104560528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2104560944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2104560528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2104560528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t>t (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2104560944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>MERGESORT ORDEN INVERSO</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$141:$A$145</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>31250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$141:$B$145</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>641</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7198</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>158785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-83ED-4B65-BD18-55AA702C140A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2068344192"/>
+        <c:axId val="2068339200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2068344192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2068339200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2068339200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> t (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2068344192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>MERGESORT ORDEN ALEATORIO</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13113648293963254"/>
+          <c:y val="0.15319444444444447"/>
+          <c:w val="0.81419685039370082"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$157:$A$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>31250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$157:$B$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1826</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7064</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33366</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>157347</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D965-458E-9B37-E29B3579CBBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2068342944"/>
+        <c:axId val="2068343360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2068342944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2068343360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2068343360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2068342944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3158,6 +4437,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5739,6 +7138,1554 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6472,6 +9419,96 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Gráfico 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6737,25 +9774,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6778,7 +9815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -6805,7 +9842,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2000</v>
       </c>
@@ -6832,7 +9869,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4000</v>
       </c>
@@ -6859,7 +9896,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8000</v>
       </c>
@@ -6886,12 +9923,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -6902,7 +9939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1000</v>
       </c>
@@ -6913,7 +9950,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2000</v>
       </c>
@@ -6924,7 +9961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4000</v>
       </c>
@@ -6935,7 +9972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8000</v>
       </c>
@@ -6946,12 +9983,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -6959,7 +9996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20</v>
       </c>
@@ -6967,7 +10004,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>21</v>
       </c>
@@ -6975,7 +10012,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>22</v>
       </c>
@@ -6983,7 +10020,7 @@
         <v>2917</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>23</v>
       </c>
@@ -6991,7 +10028,7 @@
         <v>5808</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>24</v>
       </c>
@@ -6999,7 +10036,7 @@
         <v>11690</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>25</v>
       </c>
@@ -7007,7 +10044,7 @@
         <v>23844</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>26</v>
       </c>
@@ -7015,7 +10052,7 @@
         <v>47128</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>27</v>
       </c>
@@ -7023,7 +10060,7 @@
         <v>93344</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>28</v>
       </c>
@@ -7031,7 +10068,7 @@
         <v>187000</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>29</v>
       </c>
@@ -7039,12 +10076,12 @@
         <v>374446</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -7055,7 +10092,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>20</v>
       </c>
@@ -7071,7 +10108,7 @@
         <v>26980469000.502697</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -7079,7 +10116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>80</v>
       </c>
@@ -7087,12 +10124,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -7118,7 +10155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>100</v>
       </c>
@@ -7145,7 +10182,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>200</v>
       </c>
@@ -7159,7 +10196,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>400</v>
       </c>
@@ -7173,7 +10210,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>800</v>
       </c>
@@ -7187,7 +10224,7 @@
         <v>9095</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1600</v>
       </c>
@@ -7201,7 +10238,7 @@
         <v>73426</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3200</v>
       </c>
@@ -7215,12 +10252,12 @@
         <v>659954</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -7231,7 +10268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>30</v>
       </c>
@@ -7242,7 +10279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>32</v>
       </c>
@@ -7253,7 +10290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>34</v>
       </c>
@@ -7264,7 +10301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>36</v>
       </c>
@@ -7275,7 +10312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>38</v>
       </c>
@@ -7286,7 +10323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -7300,7 +10337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>30</v>
       </c>
@@ -7316,7 +10353,7 @@
         <v>132456.01358935787</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -7324,17 +10361,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -7345,7 +10382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1000000</v>
       </c>
@@ -7356,7 +10393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2000000</v>
       </c>
@@ -7367,7 +10404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>4000000</v>
       </c>
@@ -7378,7 +10415,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>8000000</v>
       </c>
@@ -7389,7 +10426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>16000000</v>
       </c>
@@ -7400,7 +10437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>32000000</v>
       </c>
@@ -7411,7 +10448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>64000000</v>
       </c>
@@ -7420,6 +10457,234 @@
       </c>
       <c r="C101">
         <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>3</v>
+      </c>
+      <c r="B123" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>31250</v>
+      </c>
+      <c r="B124">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>62500</v>
+      </c>
+      <c r="B125">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125000</v>
+      </c>
+      <c r="B126">
+        <v>7116</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>250000</v>
+      </c>
+      <c r="B127">
+        <v>33146</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>500000</v>
+      </c>
+      <c r="B128">
+        <v>155332</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>3</v>
+      </c>
+      <c r="B140" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>31250</v>
+      </c>
+      <c r="B141">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>62500</v>
+      </c>
+      <c r="B142">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>125000</v>
+      </c>
+      <c r="B143">
+        <v>7198</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>250000</v>
+      </c>
+      <c r="B144">
+        <v>33471</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>500000</v>
+      </c>
+      <c r="B145">
+        <v>158785</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>3</v>
+      </c>
+      <c r="B156" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>31250</v>
+      </c>
+      <c r="B157">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>62500</v>
+      </c>
+      <c r="B158">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>125000</v>
+      </c>
+      <c r="B159">
+        <v>7064</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>250000</v>
+      </c>
+      <c r="B160">
+        <v>33366</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>500000</v>
+      </c>
+      <c r="B161">
+        <v>157347</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A172" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>3</v>
+      </c>
+      <c r="B173" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>250000</v>
+      </c>
+      <c r="B174">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>500000</v>
+      </c>
+      <c r="B175">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>1000000</v>
+      </c>
+      <c r="B176">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>2000000</v>
+      </c>
+      <c r="B177">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>4000000</v>
+      </c>
+      <c r="B178">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>8000000</v>
+      </c>
+      <c r="B179">
+        <v>6674</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>16000000</v>
+      </c>
+      <c r="B180">
+        <v>14779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>